<commit_message>
OrangeHRM - Complete Testcase
Testcase cover all scenarios 43/43
Total of 73 testcases
Edit requirement file location
</commit_message>
<xml_diff>
--- a/manual test/Project1 OrangeHRM/OrangeHRM manualtest document.xlsx
+++ b/manual test/Project1 OrangeHRM/OrangeHRM manualtest document.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22215" windowHeight="11730" activeTab="1"/>
+    <workbookView windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="324">
-  <si>
-    <t>FUNTIONAL REQUIREMENT</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="408">
+  <si>
+    <t>Reqirement File</t>
   </si>
   <si>
     <t>HIGH LEVEL MODULE</t>
@@ -251,13 +251,13 @@
     <t>ESS user can delete license</t>
   </si>
   <si>
-    <t>ESS user can upload attachment</t>
-  </si>
-  <si>
-    <t>ESS user can upload multiple attachments</t>
-  </si>
-  <si>
-    <t>ESS user can delete attachment</t>
+    <t>ESS user can upload attachment to qualification</t>
+  </si>
+  <si>
+    <t>ESS user can upload multiple attachments to qualification</t>
+  </si>
+  <si>
+    <t>ESS user can delete attachment from qualification</t>
   </si>
   <si>
     <t>3.1.11</t>
@@ -546,7 +546,7 @@
     <t>ESS user can add multiple Emergency Contact</t>
   </si>
   <si>
-    <t>Verify ESS user can add multiple entries emergency contact</t>
+    <t>Verify ESS user can add multiple entries to emergency contact</t>
   </si>
   <si>
     <t>1)Login to OrangeHRM as ESS
@@ -647,7 +647,7 @@
     <t>ESS user can add multiple dependent</t>
   </si>
   <si>
-    <t>Verify ESS user can add multiple entries dependent</t>
+    <t>Verify ESS user can add multiple entries to dependent</t>
   </si>
   <si>
     <t>1)Login to OrangeHRM as ESS user
@@ -694,6 +694,9 @@
     <t>Should not see selected dependent on Assigned Dependents list</t>
   </si>
   <si>
+    <t>TC_MyInfo_022</t>
+  </si>
+  <si>
     <t>Verify ESS user can not delete dependent while not selected data</t>
   </si>
   <si>
@@ -705,7 +708,7 @@
     <t>Should display an error message "please select dependent you want to delete"</t>
   </si>
   <si>
-    <t>TC_MyInfo_022</t>
+    <t>TC_MyInfo_023</t>
   </si>
   <si>
     <t>ESS user can add attachment to dependent</t>
@@ -727,6 +730,9 @@
     <t>should see data under attachments</t>
   </si>
   <si>
+    <t>TC_MyInfo_024</t>
+  </si>
+  <si>
     <t>Verify ESS user cannot add Invalid attachment to dependent</t>
   </si>
   <si>
@@ -736,7 +742,7 @@
     <t>Should display an error message "please select valid attachment"</t>
   </si>
   <si>
-    <t>TC_MyInfo_023</t>
+    <t>TC_MyInfo_025</t>
   </si>
   <si>
     <t>Verify ESS user can add immigration</t>
@@ -758,7 +764,7 @@
 </t>
   </si>
   <si>
-    <t>TC_MyInfo_024</t>
+    <t>TC_MyInfo_026</t>
   </si>
   <si>
     <t>Verify ESS user cannot add invalid immigration</t>
@@ -774,10 +780,10 @@
 "This field is required"</t>
   </si>
   <si>
-    <t>TC_MyInfo_025</t>
-  </si>
-  <si>
-    <t>Verify ESS user can add multiple entries immigration</t>
+    <t>TC_MyInfo_027</t>
+  </si>
+  <si>
+    <t>Verify ESS user can add multiple entries to immigration</t>
   </si>
   <si>
     <t>1)Login to OrangeHRM as ESS user
@@ -803,7 +809,7 @@
 as seperate records</t>
   </si>
   <si>
-    <t>TC_MyInfo_026</t>
+    <t>TC_MyInfo_028</t>
   </si>
   <si>
     <t>Verify ESS user can delete immigration</t>
@@ -821,7 +827,7 @@
     <t>Selected data should be deleted</t>
   </si>
   <si>
-    <t>TC_MyInfo_027</t>
+    <t>TC_MyInfo_029</t>
   </si>
   <si>
     <t>Verify ESS user cannot delete immigration without select data</t>
@@ -835,7 +841,7 @@
     <t>Should display an error message "please select immigration you want to delete"</t>
   </si>
   <si>
-    <t>TC_MyInfo_028</t>
+    <t>TC_MyInfo_030</t>
   </si>
   <si>
     <t>Verify ESS user can add attachment to immigration record</t>
@@ -854,7 +860,7 @@
     <t>Should see data under attachments</t>
   </si>
   <si>
-    <t>TC_MyInfo_029</t>
+    <t>TC_MyInfo_031</t>
   </si>
   <si>
     <t>ESS user can not add attachment to immigration record</t>
@@ -869,7 +875,7 @@
     <t>Should display an error message "Please select valid attachment"</t>
   </si>
   <si>
-    <t>TC_MyInfo_030</t>
+    <t>TC_MyInfo_032</t>
   </si>
   <si>
     <t>Verify ESS user can view job detail</t>
@@ -884,7 +890,7 @@
 </t>
   </si>
   <si>
-    <t>TC_MyInfo_031</t>
+    <t>TC_MyInfo_033</t>
   </si>
   <si>
     <t>Verify ESS user cannot edit job detail</t>
@@ -893,7 +899,7 @@
     <t>Textfield should be disabled</t>
   </si>
   <si>
-    <t>TC_MyInfo_032</t>
+    <t>TC_MyInfo_034</t>
   </si>
   <si>
     <t>Verify ESS user cannot see salary components</t>
@@ -903,7 +909,7 @@
 </t>
   </si>
   <si>
-    <t>TC_MyInfo_033</t>
+    <t>TC_MyInfo_035</t>
   </si>
   <si>
     <t>Verify ESS user can see the list of thier own supervisors</t>
@@ -916,7 +922,7 @@
     <t>Should display list of thier own supervisors</t>
   </si>
   <si>
-    <t>TC_MyInfo_034</t>
+    <t>TC_MyInfo_036</t>
   </si>
   <si>
     <t>Verify ESS user can see the list of thier own subordinates</t>
@@ -925,7 +931,7 @@
     <t>Should display list of thier own subordinates</t>
   </si>
   <si>
-    <t>TC_MyInfo_035</t>
+    <t>TC_MyInfo_037</t>
   </si>
   <si>
     <t>Verify ESS user can add work experience</t>
@@ -948,7 +954,7 @@
     <t>Should display data under Work Experience</t>
   </si>
   <si>
-    <t>TC_MyInfo_036</t>
+    <t>TC_MyInfo_038</t>
   </si>
   <si>
     <t>Verify ESS user cannot add invalid work experience</t>
@@ -958,10 +964,10 @@
 </t>
   </si>
   <si>
-    <t>TC_MyInfo_037</t>
-  </si>
-  <si>
-    <t>Verify ESS user can add multiple entries work experience</t>
+    <t>TC_MyInfo_039</t>
+  </si>
+  <si>
+    <t>Verify ESS user can add multiple entries to work experience</t>
   </si>
   <si>
     <t>1)Login to OrangeHRM as ESS user
@@ -989,7 +995,7 @@
     <t>Should display both data under Work Experience as seperate records</t>
   </si>
   <si>
-    <t>TC_MyInfo_038</t>
+    <t>TC_MyInfo_040</t>
   </si>
   <si>
     <t>Verify ESS user can delete work experience</t>
@@ -1008,7 +1014,7 @@
     <t>Should remove data from Work Experience</t>
   </si>
   <si>
-    <t>TC_MyInfo_039</t>
+    <t>TC_MyInfo_041</t>
   </si>
   <si>
     <t>Verify ESS user cannot delete work experience without select data</t>
@@ -1023,7 +1029,7 @@
     <t>Should display an error message "please select work experience you want to delete"</t>
   </si>
   <si>
-    <t>TC_MyInfo_040</t>
+    <t>TC_MyInfo_042</t>
   </si>
   <si>
     <t>ESS user can add education</t>
@@ -1052,7 +1058,7 @@
     <t>Should display data under Education</t>
   </si>
   <si>
-    <t>TC_MyInfo_041</t>
+    <t>TC_MyInfo_043</t>
   </si>
   <si>
     <t>ESS user cannot add invalid education</t>
@@ -1071,13 +1077,13 @@
 </t>
   </si>
   <si>
-    <t>TC_MyInfo_042</t>
+    <t>TC_MyInfo_044</t>
   </si>
   <si>
     <t>ESS user can add multiple education</t>
   </si>
   <si>
-    <t>Verify ESS user can add multiple entries education</t>
+    <t>Verify ESS user can add multiple entries to education</t>
   </si>
   <si>
     <t xml:space="preserve">1)Login to OrangeHRM as ESS user
@@ -1111,7 +1117,7 @@
 </t>
   </si>
   <si>
-    <t>TC_MyInfo_043</t>
+    <t>TC_MyInfo_045</t>
   </si>
   <si>
     <t>Verify ESS user can delete education</t>
@@ -1131,7 +1137,7 @@
     <t>Should remove data from Education</t>
   </si>
   <si>
-    <t>TC_MyInfo_044</t>
+    <t>TC_MyInfo_046</t>
   </si>
   <si>
     <t>Verify ESS user cannot delete education without select record</t>
@@ -1147,7 +1153,7 @@
 "Please select education to delete"</t>
   </si>
   <si>
-    <t>TC_MyInfo_045</t>
+    <t>TC_MyInfo_047</t>
   </si>
   <si>
     <t>Veridy ESS user can add skill</t>
@@ -1169,7 +1175,7 @@
     <t>Input data should be listed under Skills</t>
   </si>
   <si>
-    <t>TC_MyInfo_046</t>
+    <t>TC_MyInfo_048</t>
   </si>
   <si>
     <t>Veridy ESS user cannot add invalid skill</t>
@@ -1179,7 +1185,7 @@
 </t>
   </si>
   <si>
-    <t>TC_MyInfo_047</t>
+    <t>TC_MyInfo_049</t>
   </si>
   <si>
     <t>Verify ESS user can add multiple skill</t>
@@ -1207,7 +1213,7 @@
     <t>both data should be listed under Skills as seperate records</t>
   </si>
   <si>
-    <t>TC_MyInfo_048</t>
+    <t>TC_MyInfo_050</t>
   </si>
   <si>
     <t>Verify ESS user can delete skill</t>
@@ -1223,7 +1229,7 @@
     <t>Skill : SQL</t>
   </si>
   <si>
-    <t>TC_MyInfo_049</t>
+    <t>TC_MyInfo_051</t>
   </si>
   <si>
     <t>Verify ESS user cannot delete skill without select skill first</t>
@@ -1237,6 +1243,9 @@
   <si>
     <t xml:space="preserve">Should display an error mesasge "Please select skill you want to delete"
 </t>
+  </si>
+  <si>
+    <t>TC_MyInfo_052</t>
   </si>
   <si>
     <t>Verify ESS user can add language</t>
@@ -1259,12 +1268,18 @@
     <t>Input data should be listed under Language</t>
   </si>
   <si>
+    <t>TC_MyInfo_053</t>
+  </si>
+  <si>
     <t>Verify ESS user cannot add invalid language</t>
   </si>
   <si>
     <t xml:space="preserve">Should display an error message
 "This field is required" under required field that is empty
 </t>
+  </si>
+  <si>
+    <t>TC_MyInfo_054</t>
   </si>
   <si>
     <t>Verify ESS user can add multiple language</t>
@@ -1295,12 +1310,15 @@
 </t>
   </si>
   <si>
+    <t>TC_MyInfo_055</t>
+  </si>
+  <si>
     <t>Verify ESS user can delete language</t>
   </si>
   <si>
     <t xml:space="preserve">1)Login to OrangeHRM as ESS user
 2)Click on Qualification button
-3)Click Checkbox of target data under Languages
+3)Select checkbox of target data under Languages
 4)Click Delete button under Languages
 </t>
   </si>
@@ -1309,6 +1327,12 @@
   </si>
   <si>
     <t>Should remove data from Languages</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_056</t>
+  </si>
+  <si>
+    <t>Verify ESS user cannot delete language without select language first</t>
   </si>
   <si>
     <t>1)Login to OrangeHRM as ESS user
@@ -1317,6 +1341,333 @@
   </si>
   <si>
     <t xml:space="preserve">Should display an error mesasge "Please select languages you want to delete"
+</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_057</t>
+  </si>
+  <si>
+    <t>Verify ESS user can add license</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on Qualification button
+3)Click Add under License
+4)Input data
+5)Click Save button</t>
+  </si>
+  <si>
+    <t>License Type : CMA
+License Number : 78654321345678
+Issued Date : 2011-04-13
+Expiry Date : 2016-04-07</t>
+  </si>
+  <si>
+    <t>Input data should be listed under License</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_058</t>
+  </si>
+  <si>
+    <t>Verify ESS user cannot add invalid license</t>
+  </si>
+  <si>
+    <t>License Type : Null</t>
+  </si>
+  <si>
+    <t>Should display an error message
+"Plase select license type"</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_059</t>
+  </si>
+  <si>
+    <t>Verify ESS user can add multiple entries to licenses</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on Qualification button
+3)Click Add under License
+4)Input first data
+5)Click Save button
+6)Click Add under License
+7)Input second data
+8)Click Save button</t>
+  </si>
+  <si>
+    <t>License Type : CMA
+License Number : 78654321345678
+Issued Date : 2011-04-13
+Expiry Date : 2016-04-07
+License Type : Driver
+License Number : 9876543210
+Issued Date : 2010-05-11
+Expiry Date : 2015-05-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should display both data under License as seperate record
+</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_060</t>
+  </si>
+  <si>
+    <t>Verify ESS user can delete license</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on Qualification button
+3)Select checkbox of target data under License
+4)Click Delete button under license</t>
+  </si>
+  <si>
+    <t>License Type : CMA</t>
+  </si>
+  <si>
+    <t>Selected license should be removed from the list</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_061</t>
+  </si>
+  <si>
+    <t>Verify ESS user cannot delete license without select license first</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on Qualification button
+3)Click Delete button under license</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should display an error mesasge "Please select license you want to delete"
+</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_062</t>
+  </si>
+  <si>
+    <t>Verify ESS user can upload attachment to qualification</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on Qualification button
+3)Click Add button under attachment
+4)Input data to Add Attachment Form
+5)Click Upload button</t>
+  </si>
+  <si>
+    <t>File : Certs.pdf
+Comment : Null,
+File : MyCerts.pdf
+Comment : driver license</t>
+  </si>
+  <si>
+    <t>Input data should be listed under Attachments</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_063</t>
+  </si>
+  <si>
+    <t>Verify ESS user cannot upload invalid attachment to qualification</t>
+  </si>
+  <si>
+    <t>File : Null
+Comment : Null,
+File : Null
+Comment : This is my qualification</t>
+  </si>
+  <si>
+    <t>Should display an error message "Please select file"</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_064</t>
+  </si>
+  <si>
+    <t>Verify ESS user can upload multiple attachments to qualification</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on Qualification button
+3)Click Add button under attachment
+4)Input first data to Add Attachment form
+5)Click Upload button
+6)Click Add button under attachment
+7)Input second data to Add Attachment form
+8)Click Upload button</t>
+  </si>
+  <si>
+    <t>Both attachments should be list under Attachment as seperate record</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_065</t>
+  </si>
+  <si>
+    <t>Verify ESS user can delete attachment from qualification</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on Qualification button
+3)Select checkbox under Attachments
+4)Click Delete button under Attchments</t>
+  </si>
+  <si>
+    <t>File Name : Certs.docx</t>
+  </si>
+  <si>
+    <t>Selected attachment should be deleted</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_066</t>
+  </si>
+  <si>
+    <t>Verify ESS user cannot delete attachment from qualification without select any entry from Attachments</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on Qualification button
+3)Click Delete button under Attchments</t>
+  </si>
+  <si>
+    <t>Should display an error message "please select attachment you want to delete"</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_067</t>
+  </si>
+  <si>
+    <t>Verify ESS user can add membership</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on My Info
+3)Click on Personal
+4)Click on Membership
+5)Click Add button
+6)Input Data
+7)Click Save button</t>
+  </si>
+  <si>
+    <t>Membership : AFP
+Subscription Paid By : Company
+Subscription Amount : 5500
+Currency : United States Dollar
+Suibscription Commence Date : 2009-01-06
+Subscription Renewal Date : 2013-01-06</t>
+  </si>
+  <si>
+    <t>Input data should be listed under Assigned Memberships</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_068</t>
+  </si>
+  <si>
+    <t>Verify ESS user cannot add invalid membership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should display an error mesasge "Please select membership type"
+</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_069</t>
+  </si>
+  <si>
+    <t>Verify ESS user can add multiple entries to membership</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on My Info
+3)Click on Personal
+4)Click on Membership
+5)Click Add button
+6)Input first data
+7)Click Save button
+8)Click Add button
+9)Input second data
+10)Click Save button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Membership : AFP
+Subscription Paid By : Company
+Subscription Amount : 5500
+Currency : United States Dollar
+Suibscription Commence Date : 2009-01-06
+Subscription Renewal Date : 2013-01-06
+,Membership : Gym
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should display both data under Assigned Memberships as seperate record
+</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_070</t>
+  </si>
+  <si>
+    <t>Verify ESS user can delete memberships from Assigned Memberships</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on My Info
+3)Click on Personal
+4)Click on Membership
+5)Select checkbox under Assigined Membership
+6)Click Delete button</t>
+  </si>
+  <si>
+    <t>Membership : AFP</t>
+  </si>
+  <si>
+    <t>Selected membership should be deleted</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_071</t>
+  </si>
+  <si>
+    <t>Verify ESS user cannot delete memberships from Assigned Memberships without select any entry from Assigned Memberships</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on My Info
+3)Click on Personal
+4)Click on Membership
+5)Click Delete button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should display an error mesasge "Please select membership"
+</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_072</t>
+  </si>
+  <si>
+    <t>Verify ESS user can add attachment under memberships</t>
+  </si>
+  <si>
+    <t>1)Login to OrangeHRM as ESS user
+2)Click on My Info
+3)Click on Personal
+4)Click on Membership
+5)Click Add button under Attachment
+6)Select File
+7)Click Upload button</t>
+  </si>
+  <si>
+    <t>File : Membership.pdf</t>
+  </si>
+  <si>
+    <t>Input data should be listed under attachments</t>
+  </si>
+  <si>
+    <t>TC_MyInfo_073</t>
+  </si>
+  <si>
+    <t>Verify ESS user cannot add invalid attachment under memberships</t>
+  </si>
+  <si>
+    <t>File: Membership.exe
+File : NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should display one of error mesasges "Please select attachment",
+"Please select valid attachment"
 </t>
   </si>
 </sst>
@@ -1973,7 +2324,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1981,7 +2332,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2014,23 +2365,38 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2057,6 +2423,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2349,7 +2724,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>123190</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2382,16 +2757,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>685165</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>153035</xdr:rowOff>
+      <xdr:rowOff>105410</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2408,8 +2783,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3954145" y="9525"/>
-          <a:ext cx="4057650" cy="2134235"/>
+          <a:off x="2581910" y="9525"/>
+          <a:ext cx="4115435" cy="2134235"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2426,12 +2801,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>130810</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>13335</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>172720</xdr:colOff>
+      <xdr:colOff>170815</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -2450,8 +2825,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9525" y="2483485"/>
-          <a:ext cx="6860540" cy="3841115"/>
+          <a:off x="9525" y="2642235"/>
+          <a:ext cx="6858635" cy="3777615"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2725,10 +3100,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2741,194 +3116,202 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+    </row>
+    <row r="3" ht="18" spans="1:14">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+    </row>
+    <row r="12" ht="18" spans="1:14">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="3" t="s">
@@ -2943,10 +3326,10 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="3"/>
@@ -2959,136 +3342,136 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="11:14">
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
     </row>
     <row r="16" spans="11:14">
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
     </row>
     <row r="17" spans="11:14">
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
     </row>
     <row r="18" spans="11:14">
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
     </row>
     <row r="19" spans="11:14">
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
     </row>
     <row r="20" spans="11:14">
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
     </row>
     <row r="21" spans="11:14">
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
     </row>
     <row r="22" spans="11:14">
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
     </row>
     <row r="23" spans="11:14">
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
     </row>
     <row r="24" spans="11:14">
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
     </row>
     <row r="25" spans="11:14">
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
     </row>
     <row r="26" spans="11:14">
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
     </row>
     <row r="27" spans="11:14">
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
     </row>
     <row r="28" spans="11:14">
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="34"/>
     </row>
     <row r="29" spans="11:14">
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
     </row>
     <row r="30" spans="11:14">
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
     </row>
     <row r="31" spans="11:14">
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
     </row>
     <row r="32" spans="11:14">
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
     </row>
     <row r="33" spans="11:14">
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
     </row>
     <row r="34" spans="11:14">
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
-      <c r="N34" s="28"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
     </row>
     <row r="35" spans="11:14">
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="28"/>
-      <c r="N35" s="28"/>
+      <c r="K35" s="34"/>
+      <c r="L35" s="34"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="34"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="3" t="s">
@@ -3155,17 +3538,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="F36:J36"/>
     <mergeCell ref="A39:I39"/>
     <mergeCell ref="A1:D12"/>
-    <mergeCell ref="E1:J12"/>
     <mergeCell ref="A13:J14"/>
-    <mergeCell ref="K1:N35"/>
+    <mergeCell ref="K4:O11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K1:N35" r:id="rId2" display="FUNTIONAL REQUIREMENT"/>
+    <hyperlink ref="K4:O11" r:id="rId2" display="Reqirement File"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3179,25 +3561,25 @@
   <sheetPr/>
   <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="9" style="19"/>
-    <col min="3" max="3" width="52.4083333333333" style="20" customWidth="1"/>
-    <col min="4" max="4" width="16.975" style="21" customWidth="1"/>
+    <col min="1" max="2" width="9" style="24"/>
+    <col min="3" max="3" width="52.4083333333333" style="25" customWidth="1"/>
+    <col min="4" max="4" width="16.975" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="27" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -3205,993 +3587,1013 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="23">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="23">
+      <c r="A3" s="28">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="23">
+      <c r="A4" s="28">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="23">
+      <c r="A5" s="28">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="23">
+      <c r="A6" s="28">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="23">
+      <c r="A7" s="28">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="23">
+      <c r="A8" s="28">
         <v>7</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="23">
+      <c r="A9" s="28">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="23">
+      <c r="A10" s="28">
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="23">
+      <c r="A11" s="28">
         <v>10</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="23">
+      <c r="A12" s="28">
         <v>11</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="23">
+      <c r="A13" s="28">
         <v>12</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="23">
+      <c r="A14" s="28">
         <v>13</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="23">
+      <c r="A15" s="28">
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="23">
+      <c r="A16" s="28">
         <v>15</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="23">
+      <c r="A17" s="28">
         <v>16</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="23">
+      <c r="A18" s="28">
         <v>17</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="23">
+      <c r="A19" s="28">
         <v>18</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="23">
+      <c r="A20" s="28">
         <v>19</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="23">
+      <c r="A21" s="28">
         <v>20</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="23">
+      <c r="A22" s="28">
         <v>21</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="23">
+      <c r="A23" s="28">
         <v>22</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="23">
+      <c r="A24" s="28">
         <v>23</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="23">
+      <c r="A25" s="28">
         <v>24</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="23">
+      <c r="A26" s="28">
         <v>25</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="23">
+      <c r="A27" s="28">
         <v>26</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="23">
+      <c r="A28" s="28">
         <v>27</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="23">
+      <c r="A29" s="28">
         <v>28</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="23">
+      <c r="A30" s="28">
         <v>29</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="23">
+      <c r="A31" s="28">
         <v>30</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="23">
+      <c r="A32" s="28">
         <v>31</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="23">
+      <c r="A33" s="28">
         <v>32</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="23">
+      <c r="A34" s="28">
         <v>33</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="23">
+      <c r="A35" s="28">
         <v>34</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D35" s="14"/>
+      <c r="D35" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="23">
+      <c r="A36" s="28">
         <v>35</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="14"/>
+      <c r="D36" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="23">
+      <c r="A37" s="28">
         <v>36</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="14"/>
+      <c r="D37" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="23">
+      <c r="A38" s="28">
         <v>37</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="14"/>
+      <c r="D38" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="23">
+      <c r="A39" s="28">
         <v>38</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="14"/>
+      <c r="D39" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="23">
+      <c r="A40" s="28">
         <v>39</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="14"/>
+      <c r="D40" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="23">
+      <c r="A41" s="28">
         <v>40</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D41" s="14"/>
+      <c r="D41" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="23">
+      <c r="A42" s="28">
         <v>41</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="14"/>
+      <c r="D42" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="23">
+      <c r="A43" s="28">
         <v>42</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="14"/>
+      <c r="D43" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="23">
+      <c r="A44" s="28">
         <v>43</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D44" s="14"/>
+      <c r="D44" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="23"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="25" t="s">
+      <c r="A45" s="28"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="26">
+      <c r="D45" s="31">
         <f>SUM(D2:D44)</f>
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="27"/>
+      <c r="A46" s="32"/>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="27"/>
+      <c r="A47" s="32"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="27"/>
+      <c r="A48" s="32"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="27"/>
+      <c r="A49" s="32"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="27"/>
+      <c r="A50" s="32"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="27"/>
+      <c r="A51" s="32"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="27"/>
+      <c r="A52" s="32"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="27"/>
+      <c r="A53" s="32"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="27"/>
+      <c r="A54" s="32"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="27"/>
+      <c r="A55" s="32"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="27"/>
+      <c r="A56" s="32"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="27"/>
+      <c r="A57" s="32"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="27"/>
+      <c r="A58" s="32"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="27"/>
+      <c r="A59" s="32"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="27"/>
+      <c r="A60" s="32"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="27"/>
+      <c r="A61" s="32"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="27"/>
+      <c r="A62" s="32"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="27"/>
+      <c r="A63" s="32"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="27"/>
+      <c r="A64" s="32"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="27"/>
+      <c r="A65" s="32"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="27"/>
+      <c r="A66" s="32"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="27"/>
+      <c r="A67" s="32"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="27"/>
+      <c r="A68" s="32"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="27"/>
+      <c r="A69" s="32"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="27"/>
+      <c r="A70" s="32"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="27"/>
+      <c r="A71" s="32"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="27"/>
+      <c r="A72" s="32"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="27"/>
+      <c r="A73" s="32"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="27"/>
+      <c r="A74" s="32"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="27"/>
+      <c r="A75" s="32"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="27"/>
+      <c r="A76" s="32"/>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="27"/>
+      <c r="A77" s="32"/>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="27"/>
+      <c r="A78" s="32"/>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="27"/>
+      <c r="A79" s="32"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="27"/>
+      <c r="A80" s="32"/>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="27"/>
+      <c r="A81" s="32"/>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="27"/>
+      <c r="A82" s="32"/>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="27"/>
+      <c r="A83" s="32"/>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="27"/>
+      <c r="A84" s="32"/>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="27"/>
+      <c r="A85" s="32"/>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="27"/>
+      <c r="A86" s="32"/>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="27"/>
+      <c r="A87" s="32"/>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="27"/>
+      <c r="A88" s="32"/>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="27"/>
+      <c r="A89" s="32"/>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="27"/>
+      <c r="A90" s="32"/>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="27"/>
+      <c r="A91" s="32"/>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="27"/>
+      <c r="A92" s="32"/>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="27"/>
+      <c r="A93" s="32"/>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="27"/>
+      <c r="A94" s="32"/>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="27"/>
+      <c r="A95" s="32"/>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="27"/>
+      <c r="A96" s="32"/>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="27"/>
+      <c r="A97" s="32"/>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="27"/>
+      <c r="A98" s="32"/>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="27"/>
+      <c r="A99" s="32"/>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="27"/>
+      <c r="A100" s="32"/>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="27"/>
+      <c r="A101" s="32"/>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="27"/>
+      <c r="A102" s="32"/>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="27"/>
+      <c r="A103" s="32"/>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="27"/>
+      <c r="A104" s="32"/>
     </row>
     <row r="105" spans="1:1">
-      <c r="A105" s="27"/>
+      <c r="A105" s="32"/>
     </row>
     <row r="106" spans="1:1">
-      <c r="A106" s="27"/>
+      <c r="A106" s="32"/>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" s="27"/>
+      <c r="A107" s="32"/>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108" s="27"/>
+      <c r="A108" s="32"/>
     </row>
     <row r="109" spans="1:1">
-      <c r="A109" s="27"/>
+      <c r="A109" s="32"/>
     </row>
     <row r="110" spans="1:1">
-      <c r="A110" s="27"/>
+      <c r="A110" s="32"/>
     </row>
     <row r="111" spans="1:1">
-      <c r="A111" s="27"/>
+      <c r="A111" s="32"/>
     </row>
     <row r="112" spans="1:1">
-      <c r="A112" s="27"/>
+      <c r="A112" s="32"/>
     </row>
     <row r="113" spans="1:1">
-      <c r="A113" s="27"/>
+      <c r="A113" s="32"/>
     </row>
     <row r="114" spans="1:1">
-      <c r="A114" s="27"/>
+      <c r="A114" s="32"/>
     </row>
     <row r="115" spans="1:1">
-      <c r="A115" s="27"/>
+      <c r="A115" s="32"/>
     </row>
     <row r="116" spans="1:1">
-      <c r="A116" s="27"/>
+      <c r="A116" s="32"/>
     </row>
     <row r="117" spans="1:1">
-      <c r="A117" s="27"/>
+      <c r="A117" s="32"/>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="27"/>
+      <c r="A118" s="32"/>
     </row>
     <row r="119" spans="1:1">
-      <c r="A119" s="27"/>
+      <c r="A119" s="32"/>
     </row>
     <row r="120" spans="1:1">
-      <c r="A120" s="27"/>
+      <c r="A120" s="32"/>
     </row>
     <row r="121" spans="1:1">
-      <c r="A121" s="27"/>
+      <c r="A121" s="32"/>
     </row>
     <row r="122" spans="1:1">
-      <c r="A122" s="27"/>
+      <c r="A122" s="32"/>
     </row>
     <row r="123" spans="1:1">
-      <c r="A123" s="27"/>
+      <c r="A123" s="32"/>
     </row>
     <row r="124" spans="1:1">
-      <c r="A124" s="27"/>
+      <c r="A124" s="32"/>
     </row>
     <row r="125" spans="1:1">
-      <c r="A125" s="27"/>
+      <c r="A125" s="32"/>
     </row>
     <row r="126" spans="1:1">
-      <c r="A126" s="27"/>
+      <c r="A126" s="32"/>
     </row>
     <row r="127" spans="1:1">
-      <c r="A127" s="27"/>
+      <c r="A127" s="32"/>
     </row>
     <row r="128" spans="1:1">
-      <c r="A128" s="27"/>
+      <c r="A128" s="32"/>
     </row>
     <row r="129" spans="1:1">
-      <c r="A129" s="27"/>
+      <c r="A129" s="32"/>
     </row>
     <row r="130" spans="1:1">
-      <c r="A130" s="27"/>
+      <c r="A130" s="32"/>
     </row>
     <row r="131" spans="1:1">
-      <c r="A131" s="27"/>
+      <c r="A131" s="32"/>
     </row>
     <row r="132" spans="1:1">
-      <c r="A132" s="27"/>
+      <c r="A132" s="32"/>
     </row>
     <row r="133" spans="1:1">
-      <c r="A133" s="27"/>
+      <c r="A133" s="32"/>
     </row>
     <row r="134" spans="1:1">
-      <c r="A134" s="27"/>
+      <c r="A134" s="32"/>
     </row>
     <row r="135" spans="1:1">
-      <c r="A135" s="27"/>
+      <c r="A135" s="32"/>
     </row>
     <row r="136" spans="1:1">
-      <c r="A136" s="27"/>
+      <c r="A136" s="32"/>
     </row>
     <row r="137" spans="1:1">
-      <c r="A137" s="27"/>
+      <c r="A137" s="32"/>
     </row>
     <row r="138" spans="1:1">
-      <c r="A138" s="27"/>
+      <c r="A138" s="32"/>
     </row>
     <row r="139" spans="1:1">
-      <c r="A139" s="27"/>
+      <c r="A139" s="32"/>
     </row>
     <row r="140" spans="1:1">
-      <c r="A140" s="27"/>
+      <c r="A140" s="32"/>
     </row>
     <row r="141" spans="1:1">
-      <c r="A141" s="27"/>
+      <c r="A141" s="32"/>
     </row>
     <row r="142" spans="1:1">
-      <c r="A142" s="27"/>
+      <c r="A142" s="32"/>
     </row>
     <row r="143" spans="1:1">
-      <c r="A143" s="27"/>
+      <c r="A143" s="32"/>
     </row>
     <row r="144" spans="1:1">
-      <c r="A144" s="27"/>
+      <c r="A144" s="32"/>
     </row>
     <row r="145" spans="1:1">
-      <c r="A145" s="27"/>
+      <c r="A145" s="32"/>
     </row>
     <row r="146" spans="1:1">
-      <c r="A146" s="27"/>
+      <c r="A146" s="32"/>
     </row>
     <row r="147" spans="1:1">
-      <c r="A147" s="27"/>
+      <c r="A147" s="32"/>
     </row>
     <row r="148" spans="1:1">
-      <c r="A148" s="27"/>
+      <c r="A148" s="32"/>
     </row>
     <row r="149" spans="1:1">
-      <c r="A149" s="27"/>
+      <c r="A149" s="32"/>
     </row>
     <row r="150" spans="1:1">
-      <c r="A150" s="27"/>
+      <c r="A150" s="32"/>
     </row>
     <row r="151" spans="1:1">
-      <c r="A151" s="27"/>
+      <c r="A151" s="32"/>
     </row>
     <row r="152" spans="1:1">
-      <c r="A152" s="27"/>
+      <c r="A152" s="32"/>
     </row>
     <row r="153" spans="1:1">
-      <c r="A153" s="27"/>
+      <c r="A153" s="32"/>
     </row>
     <row r="154" spans="1:1">
-      <c r="A154" s="27"/>
+      <c r="A154" s="32"/>
     </row>
     <row r="155" spans="1:1">
-      <c r="A155" s="27"/>
+      <c r="A155" s="32"/>
     </row>
     <row r="156" spans="1:1">
-      <c r="A156" s="27"/>
+      <c r="A156" s="32"/>
     </row>
     <row r="157" spans="1:1">
-      <c r="A157" s="27"/>
+      <c r="A157" s="32"/>
     </row>
     <row r="158" spans="1:1">
-      <c r="A158" s="27"/>
+      <c r="A158" s="32"/>
     </row>
     <row r="159" spans="1:1">
-      <c r="A159" s="27"/>
+      <c r="A159" s="32"/>
     </row>
     <row r="160" spans="1:1">
-      <c r="A160" s="27"/>
+      <c r="A160" s="32"/>
     </row>
     <row r="161" spans="1:1">
-      <c r="A161" s="27"/>
+      <c r="A161" s="32"/>
     </row>
     <row r="162" spans="1:1">
-      <c r="A162" s="27"/>
+      <c r="A162" s="32"/>
     </row>
     <row r="163" spans="1:1">
-      <c r="A163" s="27"/>
+      <c r="A163" s="32"/>
     </row>
     <row r="164" spans="1:1">
-      <c r="A164" s="27"/>
+      <c r="A164" s="32"/>
     </row>
     <row r="165" spans="1:1">
-      <c r="A165" s="27"/>
+      <c r="A165" s="32"/>
     </row>
     <row r="166" spans="1:1">
-      <c r="A166" s="27"/>
+      <c r="A166" s="32"/>
     </row>
     <row r="167" spans="1:1">
-      <c r="A167" s="27"/>
+      <c r="A167" s="32"/>
     </row>
     <row r="168" spans="1:1">
-      <c r="A168" s="27"/>
+      <c r="A168" s="32"/>
     </row>
     <row r="169" spans="1:1">
-      <c r="A169" s="27"/>
+      <c r="A169" s="32"/>
     </row>
     <row r="170" spans="1:1">
-      <c r="A170" s="27"/>
+      <c r="A170" s="32"/>
     </row>
     <row r="171" spans="1:1">
-      <c r="A171" s="27"/>
+      <c r="A171" s="32"/>
     </row>
     <row r="172" spans="1:1">
-      <c r="A172" s="27"/>
+      <c r="A172" s="32"/>
     </row>
     <row r="173" spans="1:1">
-      <c r="A173" s="27"/>
+      <c r="A173" s="32"/>
     </row>
     <row r="174" spans="1:1">
-      <c r="A174" s="27"/>
+      <c r="A174" s="32"/>
     </row>
     <row r="175" spans="1:1">
-      <c r="A175" s="27"/>
+      <c r="A175" s="32"/>
     </row>
     <row r="176" spans="1:1">
-      <c r="A176" s="27"/>
+      <c r="A176" s="32"/>
     </row>
     <row r="177" spans="1:1">
-      <c r="A177" s="27"/>
+      <c r="A177" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4204,8 +4606,8 @@
   <sheetPr/>
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -4251,10 +4653,10 @@
       <c r="I1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4912,7 +5314,9 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="71.25" spans="1:11">
-      <c r="A23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>178</v>
+      </c>
       <c r="B23" s="5" t="s">
         <v>82</v>
       </c>
@@ -4923,26 +5327,26 @@
         <v>173</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>90</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="99.75" spans="1:11">
       <c r="A24" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>82</v>
@@ -4951,28 +5355,30 @@
         <v>30</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
     <row r="25" s="1" customFormat="1" ht="99.75" spans="1:11">
-      <c r="A25" s="5"/>
+      <c r="A25" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="B25" s="5" t="s">
         <v>82</v>
       </c>
@@ -4980,29 +5386,29 @@
         <v>30</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>90</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
     <row r="26" s="1" customFormat="1" ht="85.5" spans="1:11">
       <c r="A26" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>82</v>
@@ -5014,26 +5420,26 @@
         <v>36</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
     <row r="27" s="1" customFormat="1" ht="85.5" spans="1:11">
       <c r="A27" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>82</v>
@@ -5045,26 +5451,26 @@
         <v>36</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>90</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
     <row r="28" s="1" customFormat="1" ht="171" spans="1:11">
       <c r="A28" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>82</v>
@@ -5076,26 +5482,26 @@
         <v>37</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
     <row r="29" s="1" customFormat="1" ht="99.75" spans="1:11">
       <c r="A29" s="5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>82</v>
@@ -5107,26 +5513,26 @@
         <v>38</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
     <row r="30" s="1" customFormat="1" ht="71.25" spans="1:11">
       <c r="A30" s="5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>82</v>
@@ -5138,26 +5544,26 @@
         <v>38</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>90</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H30" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
     <row r="31" s="1" customFormat="1" ht="99.75" spans="1:11">
       <c r="A31" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>82</v>
@@ -5169,26 +5575,26 @@
         <v>39</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
     <row r="32" s="1" customFormat="1" ht="99.75" spans="1:11">
       <c r="A32" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>82</v>
@@ -5197,29 +5603,29 @@
         <v>35</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>90</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
     <row r="33" s="1" customFormat="1" ht="128.25" spans="1:11">
       <c r="A33" s="5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>82</v>
@@ -5231,26 +5637,26 @@
         <v>41</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
     <row r="34" s="1" customFormat="1" ht="42.75" spans="1:11">
       <c r="A34" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>82</v>
@@ -5262,26 +5668,26 @@
         <v>41</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="42.75" spans="1:11">
       <c r="A35" s="5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>82</v>
@@ -5293,26 +5699,26 @@
         <v>43</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
     <row r="36" s="1" customFormat="1" ht="42.75" spans="1:11">
       <c r="A36" s="5" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>82</v>
@@ -5324,26 +5730,26 @@
         <v>45</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
     <row r="37" s="1" customFormat="1" ht="42.75" spans="1:11">
       <c r="A37" s="5" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>82</v>
@@ -5355,26 +5761,26 @@
         <v>45</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H37" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
     <row r="38" s="1" customFormat="1" ht="99.75" spans="1:11">
       <c r="A38" s="5" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>82</v>
@@ -5386,26 +5792,26 @@
         <v>47</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
     <row r="39" ht="99.75" spans="1:11">
       <c r="A39" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>82</v>
@@ -5417,16 +5823,16 @@
         <v>47</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>90</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>165</v>
@@ -5436,7 +5842,7 @@
     </row>
     <row r="40" ht="156.75" spans="1:11">
       <c r="A40" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>82</v>
@@ -5448,26 +5854,26 @@
         <v>48</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
+        <v>254</v>
+      </c>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
     </row>
     <row r="41" ht="99.75" spans="1:11">
       <c r="A41" s="5" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>82</v>
@@ -5479,26 +5885,26 @@
         <v>49</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>84</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
+        <v>259</v>
+      </c>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
     </row>
     <row r="42" ht="71.25" spans="1:11">
       <c r="A42" s="5" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>82</v>
@@ -5510,26 +5916,26 @@
         <v>49</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>90</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="J42" s="16"/>
-      <c r="K42" s="16"/>
+        <v>263</v>
+      </c>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
     </row>
     <row r="43" ht="114" spans="1:11">
       <c r="A43" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>82</v>
@@ -5537,30 +5943,30 @@
       <c r="C43" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>263</v>
+      <c r="D43" s="5" t="s">
+        <v>265</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="F43" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="F43" s="13" t="s">
         <v>84</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
+        <v>269</v>
+      </c>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
     </row>
     <row r="44" ht="114" spans="1:11">
       <c r="A44" s="5" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>82</v>
@@ -5568,30 +5974,30 @@
       <c r="C44" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="F44" s="14" t="s">
+      <c r="D44" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F44" s="13" t="s">
         <v>90</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="J44" s="16"/>
-      <c r="K44" s="16"/>
+        <v>273</v>
+      </c>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
     </row>
     <row r="45" ht="199.5" spans="1:11">
       <c r="A45" s="5" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>82</v>
@@ -5600,29 +6006,29 @@
         <v>46</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="F45" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="F45" s="13" t="s">
         <v>84</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="J45" s="16"/>
-      <c r="K45" s="16"/>
+        <v>279</v>
+      </c>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
     </row>
     <row r="46" ht="114" spans="1:11">
       <c r="A46" s="5" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>82</v>
@@ -5630,30 +6036,30 @@
       <c r="C46" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F46" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="F46" s="13" t="s">
         <v>84</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="J46" s="16"/>
-      <c r="K46" s="16"/>
+        <v>284</v>
+      </c>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
     </row>
     <row r="47" ht="85.5" spans="1:11">
       <c r="A47" s="5" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B47" s="12" t="s">
         <v>82</v>
@@ -5661,30 +6067,30 @@
       <c r="C47" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="F47" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="F47" s="13" t="s">
         <v>90</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="H47" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="J47" s="16"/>
-      <c r="K47" s="16"/>
+        <v>288</v>
+      </c>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
     </row>
     <row r="48" ht="99.75" spans="1:11">
       <c r="A48" s="5" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>82</v>
@@ -5696,26 +6102,26 @@
         <v>53</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="F48" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="F48" s="13" t="s">
         <v>84</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="J48" s="16"/>
-      <c r="K48" s="16"/>
+        <v>293</v>
+      </c>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
     </row>
     <row r="49" ht="99.75" spans="1:11">
       <c r="A49" s="5" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>82</v>
@@ -5727,26 +6133,26 @@
         <v>53</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="F49" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="F49" s="13" t="s">
         <v>90</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="H49" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
+        <v>296</v>
+      </c>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
     </row>
     <row r="50" ht="142.5" spans="1:11">
       <c r="A50" s="5" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>82</v>
@@ -5754,30 +6160,30 @@
       <c r="C50" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="5" t="s">
         <v>54</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="F50" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="F50" s="13" t="s">
         <v>84</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="J50" s="16"/>
-      <c r="K50" s="16"/>
+        <v>301</v>
+      </c>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
     </row>
     <row r="51" ht="99.75" spans="1:11">
       <c r="A51" s="5" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>82</v>
@@ -5785,30 +6191,30 @@
       <c r="C51" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="F51" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="F51" s="13" t="s">
         <v>84</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="J51" s="16"/>
-      <c r="K51" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
     </row>
     <row r="52" ht="71.25" spans="1:11">
       <c r="A52" s="5" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>82</v>
@@ -5816,103 +6222,127 @@
       <c r="C52" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D52" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="F52" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="F52" s="13" t="s">
         <v>90</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="H52" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="J52" s="16"/>
-      <c r="K52" s="16"/>
-    </row>
-    <row r="53" ht="114" spans="3:11">
+        <v>309</v>
+      </c>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+    </row>
+    <row r="53" ht="114" spans="1:11">
+      <c r="A53" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="C53" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="F53" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="F53" s="13" t="s">
         <v>84</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="J53" s="16"/>
-      <c r="K53" s="16"/>
-    </row>
-    <row r="54" ht="114" spans="3:11">
+        <v>314</v>
+      </c>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+    </row>
+    <row r="54" ht="114" spans="1:11">
+      <c r="A54" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="C54" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D54" s="13" t="s">
+      <c r="D54" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E54" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G54" s="8" t="s">
         <v>312</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>309</v>
       </c>
       <c r="H54" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="J54" s="16"/>
-      <c r="K54" s="16"/>
-    </row>
-    <row r="55" ht="171" spans="3:11">
+        <v>317</v>
+      </c>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+    </row>
+    <row r="55" ht="171" spans="1:11">
+      <c r="A55" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="C55" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="F55" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="F55" s="13" t="s">
         <v>84</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="J55" s="16"/>
-      <c r="K55" s="16"/>
-    </row>
-    <row r="56" ht="114" spans="3:11">
+        <v>322</v>
+      </c>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+    </row>
+    <row r="56" ht="114" spans="1:11">
+      <c r="A56" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="C56" s="6" t="s">
         <v>46</v>
       </c>
@@ -5920,24 +6350,30 @@
         <v>58</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="F56" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="F56" s="13" t="s">
         <v>84</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16"/>
-    </row>
-    <row r="57" ht="71.25" spans="3:11">
+        <v>327</v>
+      </c>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+    </row>
+    <row r="57" ht="71.25" spans="1:11">
+      <c r="A57" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="C57" s="6" t="s">
         <v>46</v>
       </c>
@@ -5945,200 +6381,555 @@
         <v>58</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="F57" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="F57" s="13" t="s">
         <v>90</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="H57" s="10" t="s">
         <v>103</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="J57" s="16"/>
-      <c r="K57" s="16"/>
-    </row>
-    <row r="58" spans="3:11">
+        <v>331</v>
+      </c>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15"/>
+    </row>
+    <row r="58" ht="85.5" spans="1:11">
+      <c r="A58" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="C58" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="16"/>
-    </row>
-    <row r="59" spans="3:11">
+      <c r="D58" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+    </row>
+    <row r="59" ht="85.5" spans="1:11">
+      <c r="A59" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="C59" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="10"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="16"/>
-      <c r="K59" s="16"/>
-    </row>
-    <row r="60" spans="3:11">
+      <c r="D59" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+    </row>
+    <row r="60" ht="128.25" spans="1:11">
+      <c r="A60" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="C60" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="10"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="16"/>
-      <c r="K60" s="16"/>
-    </row>
-    <row r="61" spans="3:11">
+      <c r="D60" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+    </row>
+    <row r="61" ht="99.75" spans="1:11">
+      <c r="A61" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="C61" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="16"/>
-      <c r="K61" s="16"/>
-    </row>
-    <row r="62" spans="3:11">
-      <c r="C62" s="6"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="16"/>
-      <c r="K62" s="16"/>
-    </row>
-    <row r="63" spans="3:11">
-      <c r="C63" s="6"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="16"/>
-      <c r="K63" s="16"/>
-    </row>
-    <row r="64" spans="3:11">
-      <c r="C64" s="6"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="16"/>
-      <c r="K64" s="16"/>
-    </row>
-    <row r="65" spans="3:11">
-      <c r="C65" s="6"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="10"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="16"/>
-      <c r="K65" s="16"/>
-    </row>
-    <row r="66" spans="3:11">
-      <c r="C66" s="6"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
-    </row>
-    <row r="67" spans="3:9">
-      <c r="C67" s="17"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="3:9">
-      <c r="C68" s="17"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="1"/>
-    </row>
-    <row r="69" spans="3:9">
-      <c r="C69" s="17"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="18"/>
-      <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="3:9">
-      <c r="C70" s="17"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="1"/>
-    </row>
-    <row r="71" spans="3:9">
-      <c r="C71" s="17"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="18"/>
-      <c r="I71" s="1"/>
-    </row>
-    <row r="72" spans="3:9">
-      <c r="C72" s="17"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="18"/>
-      <c r="I72" s="1"/>
-    </row>
-    <row r="73" spans="3:9">
-      <c r="C73" s="17"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="18"/>
-      <c r="I73" s="1"/>
-    </row>
-    <row r="74" spans="3:9">
-      <c r="C74" s="17"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="1"/>
-    </row>
-    <row r="75" spans="3:9">
-      <c r="C75" s="17"/>
+      <c r="D61" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="I61" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+    </row>
+    <row r="62" ht="71.25" spans="1:11">
+      <c r="A62" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I62" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="J62" s="15"/>
+      <c r="K62" s="15"/>
+    </row>
+    <row r="63" ht="114" spans="1:11">
+      <c r="A63" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="I63" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+    </row>
+    <row r="64" ht="114" spans="1:11">
+      <c r="A64" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="I64" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+    </row>
+    <row r="65" ht="185.25" spans="1:11">
+      <c r="A65" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="I65" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+    </row>
+    <row r="66" ht="99.75" spans="1:11">
+      <c r="A66" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="I66" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+    </row>
+    <row r="67" ht="71.25" spans="1:11">
+      <c r="A67" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="F67" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="H67" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I67" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="J67" s="23"/>
+      <c r="K67" s="23"/>
+    </row>
+    <row r="68" ht="114" spans="1:11">
+      <c r="A68" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="F68" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G68" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="I68" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="J68" s="23"/>
+      <c r="K68" s="23"/>
+    </row>
+    <row r="69" ht="114" spans="1:11">
+      <c r="A69" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="F69" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G69" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="H69" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I69" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="J69" s="23"/>
+      <c r="K69" s="23"/>
+    </row>
+    <row r="70" ht="156.75" spans="1:11">
+      <c r="A70" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="F70" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="H70" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="I70" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="J70" s="23"/>
+      <c r="K70" s="23"/>
+    </row>
+    <row r="71" ht="114" spans="1:11">
+      <c r="A71" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="F71" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G71" s="20" t="s">
+        <v>392</v>
+      </c>
+      <c r="H71" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="I71" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="J71" s="23"/>
+      <c r="K71" s="23"/>
+    </row>
+    <row r="72" ht="85.5" spans="1:11">
+      <c r="A72" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E72" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="F72" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G72" s="20" t="s">
+        <v>397</v>
+      </c>
+      <c r="H72" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="I72" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="J72" s="23"/>
+      <c r="K72" s="23"/>
+    </row>
+    <row r="73" ht="128.25" spans="1:11">
+      <c r="A73" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>400</v>
+      </c>
+      <c r="F73" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G73" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="H73" s="17" t="s">
+        <v>402</v>
+      </c>
+      <c r="I73" s="20" t="s">
+        <v>403</v>
+      </c>
+      <c r="J73" s="23"/>
+      <c r="K73" s="23"/>
+    </row>
+    <row r="74" ht="128.25" spans="1:11">
+      <c r="A74" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="F74" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G74" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="H74" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="I74" s="20" t="s">
+        <v>407</v>
+      </c>
+      <c r="J74" s="23"/>
+      <c r="K74" s="23"/>
+    </row>
+    <row r="75" spans="4:9">
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="G75" s="1"/>
-      <c r="H75" s="18"/>
+      <c r="H75" s="22"/>
       <c r="I75" s="1"/>
     </row>
   </sheetData>

</xml_diff>